<commit_message>
switched to input template version 3. reorg of material table, added seepage materials, moved max depth to profile line, added new seep bc sheet.
</commit_message>
<xml_diff>
--- a/inputs/slopes/input_template_MASTER.xlsx
+++ b/inputs/slopes/input_template_MASTER.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/CursorProjects/slopetools/inputs/slopes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/cursor_projects/slopetools/inputs/slopes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B742D50E-2CD6-0946-BB8E-800FAD816B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1289F6-9893-994C-AFA5-CC31A65E0735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25340" yWindow="680" windowWidth="42660" windowHeight="24340" activeTab="3" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="360" yWindow="1300" windowWidth="35620" windowHeight="25080" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -22,14 +22,14 @@
     <sheet name="non-circ" sheetId="7" r:id="rId7"/>
     <sheet name="dloads" sheetId="8" r:id="rId8"/>
     <sheet name="reinforce" sheetId="6" r:id="rId9"/>
-    <sheet name="seep bc" sheetId="10" r:id="rId10"/>
+    <sheet name="seep bc" sheetId="11" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="crack_depth">main!$D$19</definedName>
-    <definedName name="crack_depth_water">main!$D$20</definedName>
-    <definedName name="gamma_w">main!$D$18</definedName>
-    <definedName name="k">main!$D$21</definedName>
-    <definedName name="max_depth">circles!$C$2</definedName>
+    <definedName name="crack_depth">main!$D$20</definedName>
+    <definedName name="crack_depth_water">main!$D$21</definedName>
+    <definedName name="gamma_w">main!$D$19</definedName>
+    <definedName name="k">main!$D$22</definedName>
+    <definedName name="max_depth">profile!$B$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="139">
   <si>
     <t>X</t>
   </si>
@@ -120,18 +120,12 @@
     <t>Sheet</t>
   </si>
   <si>
-    <t>Required</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>profile</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>Profile lines describing the slope geometry</t>
   </si>
   <si>
@@ -144,9 +138,6 @@
     <t>piezo</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>Piezometric line to define pore pressures</t>
   </si>
   <si>
@@ -199,9 +190,6 @@
   </si>
   <si>
     <t>Non-circular failure surface</t>
-  </si>
-  <si>
-    <t>yes*</t>
   </si>
   <si>
     <t>Free</t>
@@ -450,13 +438,7 @@
     <t>Sand</t>
   </si>
   <si>
-    <t>Silt</t>
-  </si>
-  <si>
     <t>Template version:</t>
-  </si>
-  <si>
-    <t>2025.06.20</t>
   </si>
   <si>
     <t>d</t>
@@ -530,9 +512,6 @@
     <t>Distributed load set (b) is only used for rapid drawdown analysis</t>
   </si>
   <si>
-    <t>dl_top</t>
-  </si>
-  <si>
     <t>Pore presssue (u) options</t>
   </si>
   <si>
@@ -557,20 +536,50 @@
     <t>alpha</t>
   </si>
   <si>
-    <t>ho</t>
-  </si>
-  <si>
-    <t>kro</t>
-  </si>
-  <si>
     <t>Seepage</t>
+  </si>
+  <si>
+    <t>max depth defines the elevation of a horizontal line that is treated as the bottom of the profile</t>
+  </si>
+  <si>
+    <t>Head:</t>
+  </si>
+  <si>
+    <t>Specified Head #1</t>
+  </si>
+  <si>
+    <t>Specified Head #2</t>
+  </si>
+  <si>
+    <t>Specified Head #3</t>
+  </si>
+  <si>
+    <t>Exit Face</t>
+  </si>
+  <si>
+    <t>Boundary conditions for seepage analysis</t>
+  </si>
+  <si>
+    <t>seep bc</t>
+  </si>
+  <si>
+    <t>Shell</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>kr0</t>
+  </si>
+  <si>
+    <t>h0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -688,19 +697,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -741,6 +757,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -818,7 +846,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -833,9 +861,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -845,22 +870,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -875,19 +897,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -896,44 +915,81 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1033,7 +1089,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>profile!$A$2</c:f>
+              <c:f>profile!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1068,36 +1124,42 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>profile!$A$4:$A$18</c:f>
+              <c:f>profile!$A$6:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>145.30000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>170</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>590</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>profile!$B$4:$B$18</c:f>
+              <c:f>profile!$B$6:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>64</c:v>
+                  <c:v>227</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>84</c:v>
+                  <c:v>317</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>84</c:v>
+                  <c:v>317</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>227</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1114,7 +1176,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>profile!$D$2</c:f>
+              <c:f>profile!$D$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1149,36 +1211,42 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>profile!$D$4:$D$18</c:f>
+              <c:f>profile!$D$6:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>115.69999999999999</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>145.30000000000001</c:v>
+                  <c:v>280</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>320</c:v>
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>350</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>profile!$E$4:$E$18</c:f>
+              <c:f>profile!$E$6:$E$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>227</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64</c:v>
+                  <c:v>307</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64</c:v>
+                  <c:v>307</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>227</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1195,7 +1263,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>profile!$G$2</c:f>
+              <c:f>profile!$G$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1230,30 +1298,30 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>profile!$G$4:$G$18</c:f>
+              <c:f>profile!$G$6:$G$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-150</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>320</c:v>
+                  <c:v>740</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>profile!$H$4:$H$18</c:f>
+              <c:f>profile!$H$6:$H$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>227</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>227</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1270,7 +1338,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>profile!$J$2</c:f>
+              <c:f>profile!$J$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1305,19 +1373,31 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>profile!$J$4:$J$18</c:f>
+              <c:f>profile!$J$6:$J$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>-150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>740</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>profile!$K$4:$K$18</c:f>
+              <c:f>profile!$K$6:$K$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>197</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1333,7 +1413,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>profile!$M$2</c:f>
+              <c:f>profile!$M$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1368,7 +1448,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>profile!$M$4:$M$18</c:f>
+              <c:f>profile!$M$6:$M$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1377,7 +1457,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>profile!$N$4:$N$18</c:f>
+              <c:f>profile!$N$6:$N$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1396,7 +1476,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>profile!$A$20</c:f>
+              <c:f>profile!$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1431,7 +1511,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>profile!$A$22:$A$36</c:f>
+              <c:f>profile!$A$24:$A$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1440,7 +1520,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>profile!$B$22:$B$36</c:f>
+              <c:f>profile!$B$24:$B$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1459,7 +1539,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>profile!$D$20</c:f>
+              <c:f>profile!$D$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1500,7 +1580,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>profile!$D$22:$D$36</c:f>
+              <c:f>profile!$D$24:$D$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1509,7 +1589,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>profile!$E$22:$E$36</c:f>
+              <c:f>profile!$E$24:$E$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1528,7 +1608,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>profile!$G$20</c:f>
+              <c:f>profile!$G$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1569,7 +1649,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>profile!$G$22:$G$36</c:f>
+              <c:f>profile!$G$24:$G$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1578,7 +1658,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>profile!$H$22:$H$36</c:f>
+              <c:f>profile!$H$24:$H$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1597,7 +1677,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>profile!$J$20</c:f>
+              <c:f>profile!$J$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1638,7 +1718,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>profile!$J$22:$J$36</c:f>
+              <c:f>profile!$J$24:$J$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1647,7 +1727,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>profile!$K$22:$K$36</c:f>
+              <c:f>profile!$K$24:$K$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1666,7 +1746,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>profile!$M$20</c:f>
+              <c:f>profile!$M$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1707,7 +1787,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>profile!$M$22:$M$36</c:f>
+              <c:f>profile!$M$24:$M$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1716,7 +1796,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>profile!$N$22:$N$36</c:f>
+              <c:f>profile!$N$24:$N$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1769,28 +1849,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-150</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>115.69999999999999</c:v>
+                  <c:v>277.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>130.5</c:v>
+                  <c:v>315</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>150</c:v>
+                  <c:v>343.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>180</c:v>
+                  <c:v>590</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>208</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>245</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>320</c:v>
+                  <c:v>740</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1802,28 +1876,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52</c:v>
+                  <c:v>275</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>61</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70</c:v>
+                  <c:v>227</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
+                  <c:v>227</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1947,6 +2015,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>225</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1956,6 +2033,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>302</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2235,6 +2321,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>69</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2244,6 +2339,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3352,6 +3456,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>-150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>251.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>347</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>740</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3361,6 +3483,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>242</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>227</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3368,6 +3508,321 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-E672-E744-B35F-ADA82DDA9A28}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="33"/>
+          <c:order val="33"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'seep bc'!$B$2:$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Specified Head #1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'seep bc'!$B$5:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>225</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'seep bc'!$C$5:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>302</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F7F5-BD4F-9D86-33CAF4D82B84}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="34"/>
+          <c:order val="34"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'seep bc'!$E$2:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Specified Head #2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'seep bc'!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'seep bc'!$F$5:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F7F5-BD4F-9D86-33CAF4D82B84}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="35"/>
+          <c:order val="35"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'seep bc'!$H$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Specified Head #3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'seep bc'!$H$5:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'seep bc'!$I$5:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F7F5-BD4F-9D86-33CAF4D82B84}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="36"/>
+          <c:order val="36"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'seep bc'!$B$14:$C$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Exit Face</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="70000"/>
+                  <a:lumOff val="30000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="70000"/>
+                  <a:lumOff val="30000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="70000"/>
+                    <a:lumOff val="30000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'seep bc'!$B$16:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>740</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'seep bc'!$C$16:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>317</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>227</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-F7F5-BD4F-9D86-33CAF4D82B84}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3448,8 +3903,6 @@
         <c:axId val="17804623"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="150"/>
-          <c:min val="-50"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4507,10 +4960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02E090B-D957-7046-AD33-44E170F709C1}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4518,164 +4971,149 @@
     <col min="1" max="1" width="5.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
     <col min="3" max="4" width="12" style="1" customWidth="1"/>
-    <col min="5" max="5" width="30.1640625" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="32" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
-        <v>87</v>
+      <c r="A1" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
+      </c>
+      <c r="D5" s="40">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="33"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="31"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="31"/>
+      <c r="C9" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="31"/>
+        <v>21</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="31"/>
+        <v>23</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="31"/>
+        <v>38</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="31"/>
+        <v>34</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="31"/>
+        <v>36</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
+      <c r="B17" s="1"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C18" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="B18" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C19" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="1">
         <v>62.4</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C19" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0</v>
-      </c>
-    </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C20" s="15" t="s">
-        <v>68</v>
+      <c r="C20" s="14" t="s">
+        <v>65</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="1"/>
-      <c r="C21" s="15" t="s">
-        <v>97</v>
+      <c r="C21" s="14" t="s">
+        <v>64</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
@@ -4683,34 +5121,234 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1"/>
+      <c r="C22" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
     </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
+  <mergeCells count="2">
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="C7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D70E3B-79D9-514F-BFD6-AD57E2F1C97E}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{847CAF5A-5624-4041-9578-842C28E166A5}">
+  <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="4" max="4" width="4" customWidth="1"/>
+    <col min="7" max="7" width="4.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B2" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="E2" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" s="33"/>
+      <c r="H2" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="33"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="41">
+        <v>302</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="41"/>
+      <c r="H3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I3" s="41"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="3">
+        <v>-150</v>
+      </c>
+      <c r="C5" s="3">
+        <v>227</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>227</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="3">
+        <v>225</v>
+      </c>
+      <c r="C7" s="3">
+        <v>302</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="43"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="3">
+        <v>320</v>
+      </c>
+      <c r="C16" s="3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="3">
+        <v>590</v>
+      </c>
+      <c r="C17" s="3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="3">
+        <v>740</v>
+      </c>
+      <c r="C18" s="3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4720,7 +5358,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4732,10 +5370,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4436F470-A09D-8C49-9B48-FB04FA2826AC}">
-  <dimension ref="A2:N36"/>
+  <dimension ref="A2:N38"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="G7" sqref="G7:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4752,144 +5390,139 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="D2" s="34" t="s">
+      <c r="B4" s="31"/>
+      <c r="D4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="G2" s="34" t="s">
+      <c r="E4" s="31"/>
+      <c r="G4" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="34"/>
-      <c r="J2" s="34" t="s">
+      <c r="H4" s="31"/>
+      <c r="J4" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="34"/>
-      <c r="M2" s="34" t="s">
+      <c r="K4" s="31"/>
+      <c r="M4" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="34"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="N4" s="31"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>145.30000000000001</v>
-      </c>
-      <c r="B4" s="3">
-        <v>64</v>
-      </c>
-      <c r="D4" s="3">
-        <v>115.69999999999999</v>
-      </c>
-      <c r="E4" s="3">
-        <v>40</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3">
-        <v>40</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>170</v>
-      </c>
-      <c r="B5" s="3">
-        <v>84</v>
-      </c>
-      <c r="D5" s="3">
-        <v>145.30000000000001</v>
-      </c>
-      <c r="E5" s="3">
-        <v>64</v>
-      </c>
-      <c r="G5" s="3">
-        <v>320</v>
-      </c>
-      <c r="H5" s="3">
-        <v>40</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
-        <v>320</v>
+        <v>0</v>
       </c>
       <c r="B6" s="3">
-        <v>84</v>
+        <v>227</v>
       </c>
       <c r="D6" s="3">
-        <v>320</v>
+        <v>240</v>
       </c>
       <c r="E6" s="3">
-        <v>64</v>
-      </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+        <v>227</v>
+      </c>
+      <c r="G6" s="3">
+        <v>-150</v>
+      </c>
+      <c r="H6" s="3">
+        <v>227</v>
+      </c>
+      <c r="J6" s="3">
+        <v>-150</v>
+      </c>
+      <c r="K6" s="3">
+        <v>197</v>
+      </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="A7" s="3">
+        <v>270</v>
+      </c>
+      <c r="B7" s="3">
+        <v>317</v>
+      </c>
+      <c r="D7" s="3">
+        <v>280</v>
+      </c>
+      <c r="E7" s="3">
+        <v>307</v>
+      </c>
+      <c r="G7" s="3">
+        <v>740</v>
+      </c>
+      <c r="H7" s="3">
+        <v>227</v>
+      </c>
+      <c r="J7" s="3">
+        <v>740</v>
+      </c>
+      <c r="K7" s="3">
+        <v>197</v>
+      </c>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="A8" s="3">
+        <v>320</v>
+      </c>
+      <c r="B8" s="3">
+        <v>317</v>
+      </c>
+      <c r="D8" s="3">
+        <v>310</v>
+      </c>
+      <c r="E8" s="3">
+        <v>307</v>
+      </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="J8" s="3"/>
@@ -4898,10 +5531,18 @@
       <c r="N8" s="3"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="A9" s="3">
+        <v>590</v>
+      </c>
+      <c r="B9" s="3">
+        <v>227</v>
+      </c>
+      <c r="D9" s="3">
+        <v>350</v>
+      </c>
+      <c r="E9" s="3">
+        <v>227</v>
+      </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="J9" s="3"/>
@@ -5017,131 +5658,131 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+    </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="D20" s="34" t="s">
+      <c r="B22" s="31"/>
+      <c r="D22" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="34"/>
-      <c r="G20" s="34" t="s">
+      <c r="E22" s="31"/>
+      <c r="G22" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="34"/>
-      <c r="J20" s="34" t="s">
+      <c r="H22" s="31"/>
+      <c r="J22" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="K20" s="34"/>
-      <c r="M20" s="34" t="s">
+      <c r="K22" s="31"/>
+      <c r="M22" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="N20" s="34"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="N22" s="31"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="M23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N21" s="2" t="s">
+      <c r="N23" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="19"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="19"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="19"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="21"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="21"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="21"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="21"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="21"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="21"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="21"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="21"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="17"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="17"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="17"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="21"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="21"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="21"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="21"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="19"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="19"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="19"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="19"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="19"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="19"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="19"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="19"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="19"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="19"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="19"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
@@ -5251,18 +5892,42 @@
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
     </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="M22:N22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5270,10 +5935,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA88A0E-2BF5-FE49-9603-08BE4D91829B}">
-  <dimension ref="A1:V26"/>
+  <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5291,99 +5956,99 @@
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="C2" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
+      <c r="C2" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="35"/>
+      <c r="L2" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="23" t="s">
+      <c r="A3" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="I3" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="J3" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="M3" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="N3" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="K3" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="L3" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="M3" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="N3" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="O3" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="P3" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q3" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="R3" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="S3" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="T3" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="U3" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="V3" s="41" t="s">
-        <v>133</v>
+      <c r="O3" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="P3" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q3" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="R3" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="S3" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="T3" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="U3" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="V3" s="28" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
@@ -5391,19 +6056,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="C4" s="3">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E4" s="3">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F4" s="3">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G4" s="3">
         <v>30</v>
@@ -5414,7 +6079,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -5433,26 +6098,30 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="C5" s="3">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E5" s="3">
         <v>100</v>
       </c>
       <c r="F5" s="3">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="3">
+        <v>300</v>
+      </c>
+      <c r="J5" s="3">
+        <v>20</v>
+      </c>
       <c r="K5" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -5471,26 +6140,30 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C6" s="3">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E6" s="3">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="F6" s="3">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="I6" s="3">
+        <v>100</v>
+      </c>
+      <c r="J6" s="3">
+        <v>19</v>
+      </c>
       <c r="K6" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -5508,16 +6181,28 @@
       <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="3">
+        <v>127</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>32</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="K7" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
@@ -5686,150 +6371,207 @@
       <c r="U13" s="3"/>
       <c r="V13" s="3"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C17" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C18"/>
+      <c r="C18" t="s">
+        <v>75</v>
+      </c>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C19" s="7" t="s">
-        <v>90</v>
+      <c r="C19" s="24" t="s">
+        <v>104</v>
       </c>
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19"/>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C20" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D20" t="s">
-        <v>91</v>
-      </c>
+      <c r="C20"/>
+      <c r="D20"/>
       <c r="E20"/>
       <c r="F20"/>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" t="s">
-        <v>93</v>
-      </c>
+      <c r="C21" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C22"/>
-      <c r="D22"/>
+      <c r="C22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" t="s">
+        <v>87</v>
+      </c>
       <c r="E22"/>
       <c r="F22"/>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C23" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="D23"/>
+      <c r="C23" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" t="s">
+        <v>89</v>
+      </c>
       <c r="E23"/>
       <c r="F23"/>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C24" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D24" t="s">
-        <v>80</v>
-      </c>
+      <c r="C24"/>
+      <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" t="s">
-        <v>81</v>
-      </c>
+      <c r="C25" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>127</v>
+        <v>121</v>
+      </c>
+      <c r="D26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26"/>
+      <c r="F26"/>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27"/>
+      <c r="F27"/>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C28" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C2:H2"/>
     <mergeCell ref="L2:Q2"/>
     <mergeCell ref="R2:V2"/>
+    <mergeCell ref="C2:J2"/>
   </mergeCells>
-  <conditionalFormatting sqref="E4:F13">
-    <cfRule type="expression" dxfId="7" priority="8">
+  <conditionalFormatting sqref="E8:F15">
+    <cfRule type="expression" dxfId="10" priority="10">
+      <formula>$D8="cp"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:H7 G8:J15">
+    <cfRule type="expression" dxfId="9" priority="9">
+      <formula>$D4="mc"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4:N15">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>$D4="cp"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:H7 G8:J13">
-    <cfRule type="expression" dxfId="6" priority="7">
+  <conditionalFormatting sqref="O4:O15">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>$D4="mc"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:J7">
+  <conditionalFormatting sqref="P4:Q7">
     <cfRule type="expression" dxfId="5" priority="4">
       <formula>$D4="cp"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M4:N13">
+  <conditionalFormatting sqref="P8:Q15">
     <cfRule type="expression" dxfId="4" priority="5">
+      <formula>$D8="mc"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R4:V15">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$D4="cp"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O4:O13">
-    <cfRule type="expression" dxfId="3" priority="6">
-      <formula>$D4="mc"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P4:Q7">
+  <conditionalFormatting sqref="E4:F7">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>$D4="cp"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P8:Q13">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>$D8="mc"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R4:V13">
+  <conditionalFormatting sqref="I4:J7">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$D4="cp"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D13" xr:uid="{EE18A772-4B35-664E-B682-D915CEF97058}">
-      <formula1>$C$20:$C$21</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D15" xr:uid="{EE18A772-4B35-664E-B682-D915CEF97058}">
+      <formula1>$C$22:$C$23</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K4:K13" xr:uid="{829D28B8-D45C-5648-988B-473A68569983}">
-      <formula1>$C$24:$C$26</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K4:K15" xr:uid="{829D28B8-D45C-5648-988B-473A68569983}">
+      <formula1>$C$26:$C$28</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5841,7 +6583,7 @@
   <dimension ref="A2:E20"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5850,14 +6592,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="36"/>
-      <c r="D2" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="E2" s="37"/>
+      <c r="A2" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="D2" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -5875,81 +6617,97 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
-        <v>0</v>
+        <v>-150</v>
       </c>
       <c r="B4" s="3">
-        <v>40</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+        <v>302</v>
+      </c>
+      <c r="D4" s="3">
+        <v>-150</v>
+      </c>
+      <c r="E4" s="3">
+        <v>250</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
-        <v>115.69999999999999</v>
+        <v>277.5</v>
       </c>
       <c r="B5" s="3">
-        <v>40</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+        <v>302</v>
+      </c>
+      <c r="D5" s="3">
+        <v>251.5</v>
+      </c>
+      <c r="E5" s="3">
+        <v>250</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
-        <v>130.5</v>
+        <v>315</v>
       </c>
       <c r="B6" s="3">
-        <v>52</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+        <v>275</v>
+      </c>
+      <c r="D6" s="3">
+        <v>315</v>
+      </c>
+      <c r="E6" s="3">
+        <v>242</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
-        <v>150</v>
+        <v>343.5</v>
       </c>
       <c r="B7" s="3">
-        <v>61</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+        <v>240</v>
+      </c>
+      <c r="D7" s="3">
+        <v>347</v>
+      </c>
+      <c r="E7" s="3">
+        <v>233</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
-        <v>180</v>
+        <v>590</v>
       </c>
       <c r="B8" s="3">
-        <v>70</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+        <v>227</v>
+      </c>
+      <c r="D8" s="3">
+        <v>590</v>
+      </c>
+      <c r="E8" s="3">
+        <v>227</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
-        <v>208</v>
+        <v>740</v>
       </c>
       <c r="B9" s="3">
-        <v>76</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+        <v>227</v>
+      </c>
+      <c r="D9" s="3">
+        <v>740</v>
+      </c>
+      <c r="E9" s="3">
+        <v>227</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>245</v>
-      </c>
-      <c r="B10" s="3">
-        <v>79</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <v>320</v>
-      </c>
-      <c r="B11" s="3">
-        <v>80</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
@@ -5996,8 +6754,8 @@
       <c r="E18" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D20" s="28" t="s">
-        <v>112</v>
+      <c r="D20" s="25" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -6011,10 +6769,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE6F868-4227-8740-A8A1-4745562882FC}">
-  <dimension ref="A2:N18"/>
+  <dimension ref="A2:N16"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6024,101 +6782,123 @@
     <col min="11" max="11" width="47.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B2" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="14" t="s">
+      <c r="H2" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>100</v>
+      </c>
+      <c r="C3" s="3">
+        <v>500</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="3">
+        <v>197</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="J3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>100</v>
+      </c>
+      <c r="C4" s="3">
+        <v>500</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="3">
+        <v>182</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="J4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3">
-        <v>145</v>
-      </c>
-      <c r="C5" s="3">
-        <v>100</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="J5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="K5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3">
-        <v>145</v>
-      </c>
-      <c r="C6" s="3">
-        <v>120</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="3">
-        <v>40</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="J6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -6127,16 +6907,10 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="J7" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -6146,9 +6920,9 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -6158,9 +6932,9 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -6170,9 +6944,9 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -6182,9 +6956,9 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -6194,39 +6968,18 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <v>9</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>10</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="18" spans="11:14" x14ac:dyDescent="0.2">
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D14" xr:uid="{06E9E004-FC39-FE49-926A-912F810F5089}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D12" xr:uid="{06E9E004-FC39-FE49-926A-912F810F5089}">
+      <formula1>$J$3:$J$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D4" xr:uid="{EED2B092-B8BF-DE44-9714-123D614E8073}">
       <formula1>$J$5:$J$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -6250,20 +7003,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>17</v>
+      <c r="C2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -6271,10 +7024,10 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -6282,10 +7035,10 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -6293,10 +7046,10 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="E5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -6371,10 +7124,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7976BB56-7732-404C-B58A-55DA7F8052B3}">
-  <dimension ref="B2:P37"/>
+  <dimension ref="B2:P29"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6390,26 +7143,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B2" s="38" t="s">
-        <v>114</v>
-      </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="F2" s="38" t="s">
-        <v>115</v>
-      </c>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="J2" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="N2" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
+      <c r="B2" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="F2" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="J2" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="N2" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -6419,7 +7172,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>0</v>
@@ -6428,7 +7181,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>0</v>
@@ -6437,7 +7190,7 @@
         <v>1</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>0</v>
@@ -6446,13 +7199,19 @@
         <v>1</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="B4" s="3">
+        <v>-150</v>
+      </c>
+      <c r="C4" s="3">
+        <v>227</v>
+      </c>
+      <c r="D4" s="3">
+        <v>4680</v>
+      </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -6464,9 +7223,15 @@
       <c r="P4" s="3"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>227</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4680</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -6478,9 +7243,15 @@
       <c r="P5" s="3"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="B6" s="3">
+        <v>225</v>
+      </c>
+      <c r="C6" s="3">
+        <v>302</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -6590,26 +7361,26 @@
       <c r="P13" s="3"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B15" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="F15" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="J15" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
-      <c r="N15" s="39" t="s">
-        <v>121</v>
-      </c>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
+      <c r="B15" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="F15" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="J15" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="N15" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
@@ -6619,7 +7390,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>0</v>
@@ -6628,7 +7399,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>0</v>
@@ -6637,7 +7408,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>0</v>
@@ -6646,13 +7417,20 @@
         <v>1</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="B17" s="3">
+        <v>-150</v>
+      </c>
+      <c r="C17" s="3">
+        <v>227</v>
+      </c>
+      <c r="D17" s="3">
+        <f>23*62.4</f>
+        <v>1435.2</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -6664,9 +7442,16 @@
       <c r="P17" s="3"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3">
+        <v>227</v>
+      </c>
+      <c r="D18" s="3">
+        <f>23*62.4</f>
+        <v>1435.2</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -6678,9 +7463,15 @@
       <c r="P18" s="3"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="B19" s="3">
+        <v>69</v>
+      </c>
+      <c r="C19" s="3">
+        <v>250</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -6790,46 +7581,13 @@
       <c r="P26" s="3"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B28" s="29" t="s">
-        <v>122</v>
+      <c r="B28" s="26" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B29" s="30" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="33" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="F33" t="s">
-        <v>124</v>
-      </c>
-      <c r="G33">
-        <f>SQRT((B4-B5)^2 + (C4-C5)^2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="G34">
-        <f>G33*D4</f>
-        <v>0</v>
-      </c>
-      <c r="K34">
-        <f>G34/2</f>
-        <v>0</v>
-      </c>
-      <c r="L34">
-        <f>K34*0.63</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="G37">
-        <f>12.35/0.777</f>
-        <v>15.894465894465894</v>
-      </c>
-      <c r="J37">
-        <f>15890.957*0.629</f>
-        <v>9995.4119530000007</v>
+      <c r="B29" s="27" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -6869,30 +7627,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="G2" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="L2" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="G2" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="L2" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="Q2" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="Q2" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -6902,10 +7660,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>0</v>
@@ -6914,10 +7672,10 @@
         <v>1</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>0</v>
@@ -6926,10 +7684,10 @@
         <v>1</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>0</v>
@@ -6938,13 +7696,13 @@
         <v>1</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="V3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.2">
@@ -6965,7 +7723,7 @@
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
       <c r="V4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.2">
@@ -7131,30 +7889,30 @@
       <c r="T13" s="3"/>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B15" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="G15" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="40"/>
-      <c r="L15" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="M15" s="40"/>
-      <c r="N15" s="40"/>
-      <c r="O15" s="40"/>
-      <c r="Q15" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="R15" s="40"/>
-      <c r="S15" s="40"/>
-      <c r="T15" s="40"/>
+      <c r="B15" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="G15" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="L15" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+      <c r="Q15" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="R15" s="37"/>
+      <c r="S15" s="37"/>
+      <c r="T15" s="37"/>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
@@ -7164,10 +7922,10 @@
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>0</v>
@@ -7176,10 +7934,10 @@
         <v>1</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>0</v>
@@ -7188,10 +7946,10 @@
         <v>1</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q16" s="2" t="s">
         <v>0</v>
@@ -7200,10 +7958,10 @@
         <v>1</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.2">
@@ -7219,10 +7977,10 @@
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="19"/>
-      <c r="S17" s="19"/>
-      <c r="T17" s="19"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B18" s="3"/>
@@ -7237,10 +7995,10 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="21"/>
-      <c r="S18" s="21"/>
-      <c r="T18" s="21"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
@@ -7255,10 +8013,10 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
-      <c r="T19" s="21"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
@@ -7273,10 +8031,10 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="21"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="21"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="19"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B21" s="3"/>
@@ -7387,30 +8145,30 @@
       <c r="T26" s="3"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B28" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40"/>
-      <c r="G28" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="H28" s="40"/>
-      <c r="I28" s="40"/>
-      <c r="J28" s="40"/>
-      <c r="L28" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="M28" s="40"/>
-      <c r="N28" s="40"/>
-      <c r="O28" s="40"/>
-      <c r="Q28" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="R28" s="40"/>
-      <c r="S28" s="40"/>
-      <c r="T28" s="40"/>
+      <c r="B28" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="G28" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="L28" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="M28" s="37"/>
+      <c r="N28" s="37"/>
+      <c r="O28" s="37"/>
+      <c r="Q28" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="R28" s="37"/>
+      <c r="S28" s="37"/>
+      <c r="T28" s="37"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
@@ -7420,10 +8178,10 @@
         <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>0</v>
@@ -7432,10 +8190,10 @@
         <v>1</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>0</v>
@@ -7444,10 +8202,10 @@
         <v>1</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q29" s="2" t="s">
         <v>0</v>
@@ -7456,83 +8214,83 @@
         <v>1</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="T29" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B30" s="18"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="19"/>
-      <c r="S30" s="19"/>
-      <c r="T30" s="19"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
+      <c r="O30" s="17"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="17"/>
+      <c r="S30" s="17"/>
+      <c r="T30" s="17"/>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B31" s="20"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
-      <c r="O31" s="21"/>
-      <c r="Q31" s="20"/>
-      <c r="R31" s="21"/>
-      <c r="S31" s="21"/>
-      <c r="T31" s="21"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B32" s="20"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="21"/>
-      <c r="N32" s="21"/>
-      <c r="O32" s="21"/>
-      <c r="Q32" s="20"/>
-      <c r="R32" s="21"/>
-      <c r="S32" s="21"/>
-      <c r="T32" s="21"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B33" s="20"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="L33" s="20"/>
-      <c r="M33" s="21"/>
-      <c r="N33" s="21"/>
-      <c r="O33" s="21"/>
-      <c r="Q33" s="20"/>
-      <c r="R33" s="21"/>
-      <c r="S33" s="21"/>
-      <c r="T33" s="21"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B34" s="3"/>

</xml_diff>